<commit_message>
He agregado el diccionario de datos
</commit_message>
<xml_diff>
--- a/DiccionarioDeDatos.xlsx
+++ b/DiccionarioDeDatos.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/santiagobeltran/Documents/Estudios/Universidad/4Semestre/ModYSim4/TallerMod-Sim4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtjua\arturo\Mode 4\TallerMod-Sim4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E21BBA9-6D71-0340-9C84-CEDCFAE1F465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1C3EEF0-4B7F-4C4C-B9FF-B0377AF8794B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{8F694CF3-8E02-E440-B355-1B3D9C926FFD}"/>
+    <workbookView xWindow="1380" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{A9258C52-298E-49B0-9F12-BFAC7FADA24F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,12 +35,157 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>pidnum</t>
+  </si>
+  <si>
+    <t>cid</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>trt</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>wtkg</t>
+  </si>
+  <si>
+    <t>hemo</t>
+  </si>
+  <si>
+    <t>homo</t>
+  </si>
+  <si>
+    <t>drugs</t>
+  </si>
+  <si>
+    <t>karnof</t>
+  </si>
+  <si>
+    <t>race</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>symptom</t>
+  </si>
+  <si>
+    <t>treat</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>ID del paciente  </t>
+  </si>
+  <si>
+    <t>Peso del paciente (kg)</t>
+  </si>
+  <si>
+    <t>Tiene hemofilia (1 = si; 0 = no)</t>
+  </si>
+  <si>
+    <t>Es homosexual (1 = si; 0 = no)</t>
+  </si>
+  <si>
+    <t>Género (0 = mujer; 1 = hombre) </t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Índice de Karnofsky (1-100)</t>
+  </si>
+  <si>
+    <t>¿Tiene historia de uso de drogas? (0 = no; 1 = si)</t>
+  </si>
+  <si>
+    <t>Tipo de tratamiento
+0 = Zidovudina solamente
+1 = Zidovudina + Didanosina
+2 = Zidovudina + Zalcitabina
+3 = Didanosina solamente</t>
+  </si>
+  <si>
+    <t>Binario</t>
+  </si>
+  <si>
+    <t>Entero</t>
+  </si>
+  <si>
+    <t>indicador de síntomas (0 = es asintomático ; 1 = tiene síntomas)</t>
+  </si>
+  <si>
+    <t>Continuo</t>
+  </si>
+  <si>
+    <t>Tiempo de falla o censura</t>
+  </si>
+  <si>
+    <t>Indicador de tratamiento (0= Zidovudina  solamente; 1= otros)</t>
+  </si>
+  <si>
+    <t>Indicador de censura (1 = falla; 0 = censura)</t>
+  </si>
+  <si>
+    <t>Raza (0 = blanco; 1 = no) </t>
+  </si>
+  <si>
+    <t>Edad del paciente</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF303030"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -54,7 +199,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,12 +207,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -83,6 +261,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -401,13 +583,486 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EDB91FF-97A2-E842-B21E-50312AC4B0EB}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A16F28-B436-44D8-B4A1-69EBEBEF2564}">
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="58.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100123CA3431874DD4EBD37E8894C072552" ma:contentTypeVersion="16" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="d4a4eeea296414ef88e6e3db1e33fb57">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2b122bf2-d568-48f6-8792-aa43ab5f6add" xmlns:ns4="cf97cd10-e5d2-4bf2-a8ae-92e83e26609a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="966470613a61756c0b289251fd3745a6" ns3:_="" ns4:_="">
+    <xsd:import namespace="2b122bf2-d568-48f6-8792-aa43ab5f6add"/>
+    <xsd:import namespace="cf97cd10-e5d2-4bf2-a8ae-92e83e26609a"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:_activity" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2b122bf2-d568-48f6-8792-aa43ab5f6add" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="12" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="13" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_activity" ma:index="14" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSystemTags" ma:index="19" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="20" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="21" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="22" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="23" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="cf97cd10-e5d2-4bf2-a8ae-92e83e26609a" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="15" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="16" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="17" nillable="true" ma:displayName="Hash de la sugerencia para compartir" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2b122bf2-d568-48f6-8792-aa43ab5f6add" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D81FA5FF-B7E9-470E-8CD4-2DDF21CA4E8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2b122bf2-d568-48f6-8792-aa43ab5f6add"/>
+    <ds:schemaRef ds:uri="cf97cd10-e5d2-4bf2-a8ae-92e83e26609a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B862011A-0B46-4524-A852-004AAFFCEB68}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBC1C702-06BF-4052-BBA7-4807B8F3C832}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="cf97cd10-e5d2-4bf2-a8ae-92e83e26609a"/>
+    <ds:schemaRef ds:uri="2b122bf2-d568-48f6-8792-aa43ab5f6add"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
hice unas correlaciones y verifique algunos casos extremos
</commit_message>
<xml_diff>
--- a/DiccionarioDeDatos.xlsx
+++ b/DiccionarioDeDatos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtjua\arturo\Mode 4\TallerMod-Sim4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1C3EEF0-4B7F-4C4C-B9FF-B0377AF8794B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336E0AAE-0E4C-4683-BFA5-BE83ED140949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{A9258C52-298E-49B0-9F12-BFAC7FADA24F}"/>
+    <workbookView xWindow="13260" yWindow="5610" windowWidth="15540" windowHeight="9990" xr2:uid="{A9258C52-298E-49B0-9F12-BFAC7FADA24F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -261,10 +261,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -587,7 +583,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,6 +762,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100123CA3431874DD4EBD37E8894C072552" ma:contentTypeVersion="16" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="d4a4eeea296414ef88e6e3db1e33fb57">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2b122bf2-d568-48f6-8792-aa43ab5f6add" xmlns:ns4="cf97cd10-e5d2-4bf2-a8ae-92e83e26609a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="966470613a61756c0b289251fd3745a6" ns3:_="" ns4:_="">
     <xsd:import namespace="2b122bf2-d568-48f6-8792-aa43ab5f6add"/>
@@ -1006,15 +1011,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1024,6 +1020,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B862011A-0B46-4524-A852-004AAFFCEB68}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D81FA5FF-B7E9-470E-8CD4-2DDF21CA4E8C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1038,14 +1042,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B862011A-0B46-4524-A852-004AAFFCEB68}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
correcciones al diccionario de datos
</commit_message>
<xml_diff>
--- a/DiccionarioDeDatos.xlsx
+++ b/DiccionarioDeDatos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtjua\arturo\Mode 4\TallerMod-Sim4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336E0AAE-0E4C-4683-BFA5-BE83ED140949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9260B63-60A8-44EB-BE83-3A20CD6AF156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13260" yWindow="5610" windowWidth="15540" windowHeight="9990" xr2:uid="{A9258C52-298E-49B0-9F12-BFAC7FADA24F}"/>
+    <workbookView xWindow="-255" yWindow="2685" windowWidth="28620" windowHeight="12075" xr2:uid="{A9258C52-298E-49B0-9F12-BFAC7FADA24F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -104,9 +104,6 @@
     <t>Tipo</t>
   </si>
   <si>
-    <t>Índice de Karnofsky (1-100)</t>
-  </si>
-  <si>
     <t>¿Tiene historia de uso de drogas? (0 = no; 1 = si)</t>
   </si>
   <si>
@@ -135,20 +132,31 @@
     <t>Indicador de tratamiento (0= Zidovudina  solamente; 1= otros)</t>
   </si>
   <si>
-    <t>Indicador de censura (1 = falla; 0 = censura)</t>
-  </si>
-  <si>
     <t>Raza (0 = blanco; 1 = no) </t>
   </si>
   <si>
     <t>Edad del paciente</t>
+  </si>
+  <si>
+    <t>Índice de Karnofsky (1-100).
+ Es una escala que mide la capacidad de un paciente para realizar actividades de la vida diaria.
+100: Normal, sin quejas; sin evidencia de enfermedad.
+60: Requiere asistencia ocasional pero es capaz de cuidar la mayoría de sus necesidades personales.
+50: Requiere asistencia considerable y atención médica frecuente.
+40: Incapacitado para realizar la mayoría de las actividades, requiere asistencia diaria.
+0: Fallecido.</t>
+  </si>
+  <si>
+    <t>Indicador de censura (1 = falla; 0 = censura)
+Falla indica que hubo una progresión a SIDA o muerte.
+Censura indica un retiro del paciente, o no hubo un evento de interés al final del periodo de observación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,9 +191,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF303030"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -226,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -241,11 +255,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,13 +601,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A16F28-B436-44D8-B4A1-69EBEBEF2564}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -610,18 +629,18 @@
         <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>31</v>
+      <c r="B3" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -629,10 +648,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -640,10 +659,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -651,10 +670,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -665,7 +684,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -676,7 +695,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -687,29 +706,29 @@
         <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>22</v>
+      <c r="B11" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -717,10 +736,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -731,7 +750,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -739,21 +758,21 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>30</v>
+      <c r="B15" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -762,15 +781,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100123CA3431874DD4EBD37E8894C072552" ma:contentTypeVersion="16" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="d4a4eeea296414ef88e6e3db1e33fb57">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2b122bf2-d568-48f6-8792-aa43ab5f6add" xmlns:ns4="cf97cd10-e5d2-4bf2-a8ae-92e83e26609a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="966470613a61756c0b289251fd3745a6" ns3:_="" ns4:_="">
     <xsd:import namespace="2b122bf2-d568-48f6-8792-aa43ab5f6add"/>
@@ -1011,6 +1021,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1020,14 +1039,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B862011A-0B46-4524-A852-004AAFFCEB68}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D81FA5FF-B7E9-470E-8CD4-2DDF21CA4E8C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1042,6 +1053,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B862011A-0B46-4524-A852-004AAFFCEB68}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>